<commit_message>
Removed anyOf and oneOf from schemas, created a new class for file-level metadata and added a second example for each slot
</commit_message>
<xml_diff>
--- a/project/excel/bia_faim_models.xlsx
+++ b/project/excel/bia_faim_models.xlsx
@@ -11,13 +11,10 @@
     <sheet name="Publications" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Author" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="OrganisationInfo" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="OrganisationInfoCollection" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="OrganisationURL" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="FundingStatement" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="GrantReference" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="GrantReferenceCollection" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="Annotations" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="Version" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="GrantReference" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="FileLevelMetadata" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Annotations" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Version" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -423,7 +420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,7 +461,7 @@
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>funding</t>
+          <t>funding_statement</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
@@ -485,6 +482,11 @@
       <c r="K1" t="inlineStr">
         <is>
           <t>link_description</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>grants</t>
         </is>
       </c>
     </row>
@@ -494,123 +496,6 @@
       <formula1>"CC0,CC_BY"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:J1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>annotation_overview</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>annotation_type</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>annotation_method</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>annotation_criteria</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>annotation_coverage</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>source_image</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>annotation_confidence_level</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>spatial_information</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>transformatons</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>authors</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"class_labels,bounding_boxes,counts,segmentation_mask"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>version</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>timestamp</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>changes</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>previous_version</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -698,12 +583,12 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>affiliation</t>
+          <t>role</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>role</t>
+          <t>organisation</t>
         </is>
       </c>
     </row>
@@ -713,6 +598,42 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>organisation_name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>address</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>ror_id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -729,12 +650,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>organisation_name</t>
+          <t>grant_id</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>address</t>
+          <t>funder</t>
         </is>
       </c>
     </row>
@@ -743,13 +664,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -760,22 +681,47 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>organisation</t>
+          <t>annotation_id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>annotation_type</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>source_image_id</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>transformations</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>spatial_information</t>
         </is>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"class_labels,bounding_boxes,counts,derived_annotations,geometrical_annotations,graphs,point_annotations,segmentation_mask,tracks,weak_annotations,other"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -786,7 +732,37 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>ror_id</t>
+          <t>annotation_overview</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>annotation_method</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>annotation_criteria</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>annotation_coverage</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>annotation_confidence_level</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>authors</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>file_metadata</t>
         </is>
       </c>
     </row>
@@ -795,13 +771,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -812,64 +788,22 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>funding_statement</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>grant_id</t>
+          <t>version</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>funder</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>grants</t>
+          <t>timestamp</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>changes</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>previous_version</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Added a new creation time attribute for the annotations class
</commit_message>
<xml_diff>
--- a/project/excel/bia_faim_models.xlsx
+++ b/project/excel/bia_faim_models.xlsx
@@ -670,7 +670,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -702,6 +702,11 @@
       <c r="E1" t="inlineStr">
         <is>
           <t>spatial_information</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>annotation_creation_time</t>
         </is>
       </c>
     </row>

</xml_diff>